<commit_message>
Documentation / ERP Module Finished
</commit_message>
<xml_diff>
--- a/Zero.Extension.Runtime.Ambient.DB/src/main/resources/plugins/zero-extension-runtime-ambient/data/X_MENU/BANNER-zero.extra.xlsx
+++ b/Zero.Extension.Runtime.Ambient.DB/src/main/resources/plugins/zero-extension-runtime-ambient/data/X_MENU/BANNER-zero.extra.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/zero-cloud/web-app/workshop/zero-ws/zero-plugins-extension/Zero.Extension.Runtime.Ambient.DB/src/main/resources/plugins/zero-extension-runtime-ambient/data/X_MENU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7861AC3-BAD5-8D4F-9864-2DAE95276BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71AD7AB-D5D9-D142-AD52-CBCAD86ABDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-44000" yWindow="-2940" windowWidth="33320" windowHeight="15900" tabRatio="591" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,7 +117,7 @@
     <t>zero.extra.research</t>
   </si>
   <si>
-    <t>CODE:config</t>
+    <t>NAME:config</t>
   </si>
 </sst>
 </file>

</xml_diff>